<commit_message>
add ITLubberLogisticRegression based sklearn
</commit_message>
<xml_diff>
--- a/逻辑回归模型拟合效果.xlsx
+++ b/逻辑回归模型拟合效果.xlsx
@@ -635,14 +635,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="28" customWidth="1" min="1" max="1"/>
-    <col width="23" customWidth="1" min="2" max="2"/>
+    <col width="24" customWidth="1" min="2" max="2"/>
     <col width="28" customWidth="1" min="3" max="3"/>
-    <col width="28" customWidth="1" min="4" max="4"/>
+    <col width="24" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="24" customWidth="1" min="6" max="6"/>
-    <col width="23" customWidth="1" min="7" max="7"/>
-    <col width="28" customWidth="1" min="8" max="8"/>
-    <col width="27" customWidth="1" min="9" max="9"/>
+    <col width="28" customWidth="1" min="6" max="6"/>
+    <col width="28" customWidth="1" min="7" max="7"/>
+    <col width="23" customWidth="1" min="8" max="8"/>
+    <col width="28" customWidth="1" min="9" max="9"/>
     <col width="24" customWidth="1" min="10" max="10"/>
     <col width="20" customWidth="1" min="11" max="11"/>
     <col width="22" customWidth="1" min="12" max="12"/>
@@ -698,7 +698,7 @@
       </c>
       <c r="D3" s="10" t="inlineStr">
         <is>
-          <t>0.214</t>
+          <t>0.206</t>
         </is>
       </c>
       <c r="E3" s="10" t="n"/>
@@ -728,7 +728,7 @@
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>692.2317</t>
+          <t>698.9520</t>
         </is>
       </c>
       <c r="E4" s="10" t="n"/>
@@ -748,7 +748,7 @@
       </c>
       <c r="B5" s="10" t="inlineStr">
         <is>
-          <t>2022-10-27 13:19</t>
+          <t>2022-10-28 12:05</t>
         </is>
       </c>
       <c r="C5" s="10" t="inlineStr">
@@ -758,7 +758,7 @@
       </c>
       <c r="D5" s="10" t="inlineStr">
         <is>
-          <t>737.7425</t>
+          <t>744.4628</t>
         </is>
       </c>
       <c r="E5" s="10" t="n"/>
@@ -788,7 +788,7 @@
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>-336.12</t>
+          <t>-339.48</t>
         </is>
       </c>
       <c r="E6" s="10" t="n"/>
@@ -848,7 +848,7 @@
       </c>
       <c r="D8" s="10" t="inlineStr">
         <is>
-          <t>1.2096e-34</t>
+          <t>3.0601e-33</t>
         </is>
       </c>
       <c r="E8" s="10" t="n"/>
@@ -1009,155 +1009,155 @@
         </is>
       </c>
       <c r="B14" s="10" t="n">
-        <v>-0.8552601409281363</v>
+        <v>-0.8647859747157886</v>
       </c>
       <c r="C14" s="10" t="n">
-        <v>0.09762013715076218</v>
+        <v>0.09761220915841198</v>
       </c>
       <c r="D14" s="10" t="n">
-        <v>-8.76110366048035</v>
+        <v>-8.85940377921734</v>
       </c>
       <c r="E14" s="10" t="n">
-        <v>1.933478969779483e-18</v>
+        <v>8.044350457137041e-19</v>
       </c>
       <c r="F14" s="10" t="n">
-        <v>-1.046592093909491</v>
+        <v>-1.056102389117667</v>
       </c>
       <c r="G14" s="10" t="n">
-        <v>-0.6639281879467819</v>
+        <v>-0.6734695603139103</v>
       </c>
       <c r="H14" s="10" t="n">
-        <v>-1.167833424820575</v>
+        <v>-1.174718569145676</v>
       </c>
       <c r="I14" s="10" t="n">
-        <v>76.7569373496822</v>
+        <v>78.48903532321047</v>
       </c>
       <c r="J14" s="10" t="n">
-        <v>1.933478969779486e-18</v>
+        <v>8.044350457137075e-19</v>
       </c>
       <c r="K14" s="10" t="n">
-        <v>1.052584616147686</v>
+        <v>1.052162898921845</v>
       </c>
       <c r="L14" s="11" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="9" t="inlineStr">
         <is>
-          <t>housing</t>
+          <t>age.in.years</t>
         </is>
       </c>
       <c r="B15" s="10" t="n">
-        <v>0.7547975408453721</v>
+        <v>0.9184832030063913</v>
       </c>
       <c r="C15" s="10" t="n">
-        <v>0.3544314000325444</v>
+        <v>0.4031265854064456</v>
       </c>
       <c r="D15" s="10" t="n">
-        <v>2.129601216980396</v>
+        <v>2.278398984974772</v>
       </c>
       <c r="E15" s="10" t="n">
-        <v>0.03320455050447055</v>
+        <v>0.02270281682687334</v>
       </c>
       <c r="F15" s="10" t="n">
-        <v>0.06012476179147652</v>
+        <v>0.1283696143991477</v>
       </c>
       <c r="G15" s="10" t="n">
-        <v>1.449470319899268</v>
+        <v>1.708596791613635</v>
       </c>
       <c r="H15" s="10" t="n">
-        <v>0.1970774024967832</v>
+        <v>0.2228576097576813</v>
       </c>
       <c r="I15" s="10" t="n">
-        <v>4.535201343364383</v>
+        <v>5.191101934734069</v>
       </c>
       <c r="J15" s="10" t="n">
-        <v>0.03320455050447061</v>
+        <v>0.02270281682687339</v>
       </c>
       <c r="K15" s="10" t="n">
-        <v>1.029590684339555</v>
+        <v>1.073323800553426</v>
       </c>
       <c r="L15" s="11" t="n">
-        <v>0.0115662686069827</v>
+        <v>0.02884030043338393</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="9" t="inlineStr">
         <is>
-          <t>status.of.existing.checking.account</t>
+          <t>savings.account.and.bonds</t>
         </is>
       </c>
       <c r="B16" s="10" t="n">
-        <v>0.8886050794910652</v>
+        <v>0.7794882686476101</v>
       </c>
       <c r="C16" s="10" t="n">
-        <v>0.1320993996762082</v>
+        <v>0.2342894285035776</v>
       </c>
       <c r="D16" s="10" t="n">
-        <v>6.726791201694669</v>
+        <v>3.327031328840804</v>
       </c>
       <c r="E16" s="10" t="n">
-        <v>1.734453460485695e-11</v>
+        <v>0.0008777650445891572</v>
       </c>
       <c r="F16" s="10" t="n">
-        <v>0.6296950137463349</v>
+        <v>0.3202894268221261</v>
       </c>
       <c r="G16" s="10" t="n">
-        <v>1.147515145235795</v>
+        <v>1.238687110473094</v>
       </c>
       <c r="H16" s="10" t="n">
-        <v>0.7298206318757319</v>
+        <v>0.3629094401241452</v>
       </c>
       <c r="I16" s="10" t="n">
-        <v>45.2497198711968</v>
+        <v>11.0691374630882</v>
       </c>
       <c r="J16" s="10" t="n">
-        <v>1.734453460485704e-11</v>
+        <v>0.0008777650445891588</v>
       </c>
       <c r="K16" s="10" t="n">
-        <v>1.099490764492609</v>
+        <v>1.099460784554796</v>
       </c>
       <c r="L16" s="11" t="n">
-        <v>0.4128446326621481</v>
+        <v>0.08245227815188172</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="9" t="inlineStr">
         <is>
-          <t>installment.rate.in.percentage.of.disposable.income</t>
+          <t>credit.amount</t>
         </is>
       </c>
       <c r="B17" s="10" t="n">
-        <v>1.856813456658066</v>
+        <v>1.566930222688853</v>
       </c>
       <c r="C17" s="10" t="n">
-        <v>0.6355507777066449</v>
+        <v>0.4667519897280076</v>
       </c>
       <c r="D17" s="10" t="n">
-        <v>2.921581597867427</v>
+        <v>3.35709382535671</v>
       </c>
       <c r="E17" s="10" t="n">
-        <v>0.003482590366787969</v>
+        <v>0.0007876637873281963</v>
       </c>
       <c r="F17" s="10" t="n">
-        <v>0.6111568220066199</v>
+        <v>0.6521131331095487</v>
       </c>
       <c r="G17" s="10" t="n">
-        <v>3.102470091309512</v>
+        <v>2.481747312268157</v>
       </c>
       <c r="H17" s="10" t="n">
-        <v>0.2858924048967472</v>
+        <v>0.3241794841220327</v>
       </c>
       <c r="I17" s="10" t="n">
-        <v>8.53563903299759</v>
+        <v>11.27007895224815</v>
       </c>
       <c r="J17" s="10" t="n">
-        <v>0.003482590366787966</v>
+        <v>0.0007876637873281982</v>
       </c>
       <c r="K17" s="10" t="n">
-        <v>1.030029867548937</v>
+        <v>1.067056397113379</v>
       </c>
       <c r="L17" s="11" t="n">
-        <v>0.0110638710986919</v>
+        <v>0.03597733102432686</v>
       </c>
     </row>
     <row r="18">
@@ -1167,237 +1167,237 @@
         </is>
       </c>
       <c r="B18" s="10" t="n">
-        <v>1.044011624412964</v>
+        <v>1.050352108104194</v>
       </c>
       <c r="C18" s="10" t="n">
-        <v>0.2662210309938199</v>
+        <v>0.2450305212914843</v>
       </c>
       <c r="D18" s="10" t="n">
-        <v>3.921597104915424</v>
+        <v>4.286617448994086</v>
       </c>
       <c r="E18" s="10" t="n">
-        <v>8.796398570381868e-05</v>
+        <v>1.814143068280143e-05</v>
       </c>
       <c r="F18" s="10" t="n">
-        <v>0.522227991737955</v>
+        <v>0.5701011112598093</v>
       </c>
       <c r="G18" s="10" t="n">
-        <v>1.565795257087972</v>
+        <v>1.530603104948578</v>
       </c>
       <c r="H18" s="10" t="n">
-        <v>0.391289735712572</v>
+        <v>0.4314904837987295</v>
       </c>
       <c r="I18" s="10" t="n">
-        <v>15.37892385328103</v>
+        <v>18.37508915402056</v>
       </c>
       <c r="J18" s="10" t="n">
-        <v>8.796398570381875e-05</v>
+        <v>1.81414306828015e-05</v>
       </c>
       <c r="K18" s="10" t="n">
-        <v>1.053265273621899</v>
+        <v>1.048049540301305</v>
       </c>
       <c r="L18" s="11" t="n">
-        <v>0.06185777264762857</v>
+        <v>0.08167786554409695</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="9" t="inlineStr">
         <is>
-          <t>credit.amount</t>
+          <t>status.of.existing.checking.account</t>
         </is>
       </c>
       <c r="B19" s="10" t="n">
-        <v>1.18364621816148</v>
+        <v>0.8519965418544813</v>
       </c>
       <c r="C19" s="10" t="n">
-        <v>0.2437052131938017</v>
+        <v>0.1207789764483408</v>
       </c>
       <c r="D19" s="10" t="n">
-        <v>4.85687689093548</v>
+        <v>7.054179186713795</v>
       </c>
       <c r="E19" s="10" t="n">
-        <v>1.192516841007804e-06</v>
+        <v>1.73622526418799e-12</v>
       </c>
       <c r="F19" s="10" t="n">
-        <v>0.705992777456973</v>
+        <v>0.6152740979261219</v>
       </c>
       <c r="G19" s="10" t="n">
-        <v>1.661299658865987</v>
+        <v>1.088718985782841</v>
       </c>
       <c r="H19" s="10" t="n">
-        <v>0.4788897009452719</v>
+        <v>0.7503444705159771</v>
       </c>
       <c r="I19" s="10" t="n">
-        <v>23.5892531337031</v>
+        <v>49.7614439982661</v>
       </c>
       <c r="J19" s="10" t="n">
-        <v>1.192516841007802e-06</v>
+        <v>1.736225264187991e-12</v>
       </c>
       <c r="K19" s="10" t="n">
-        <v>1.030414485979162</v>
+        <v>1.123270309366261</v>
       </c>
       <c r="L19" s="11" t="n">
-        <v>0.2321361650517705</v>
+        <v>0.548968284363424</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="9" t="inlineStr">
         <is>
-          <t>age.in.years</t>
+          <t>number.of.existing.credits.at.this.bank</t>
         </is>
       </c>
       <c r="B20" s="10" t="n">
-        <v>0.73485669011017</v>
+        <v>-1.562980979090772</v>
       </c>
       <c r="C20" s="10" t="n">
-        <v>0.3896662481046385</v>
+        <v>0.9292964284272509</v>
       </c>
       <c r="D20" s="10" t="n">
-        <v>1.885861795022175</v>
+        <v>-1.681897111921515</v>
       </c>
       <c r="E20" s="10" t="n">
-        <v>0.05931358103946834</v>
+        <v>0.09258879282334444</v>
       </c>
       <c r="F20" s="10" t="n">
-        <v>-0.02887512216577059</v>
+        <v>-3.384368509769888</v>
       </c>
       <c r="G20" s="10" t="n">
-        <v>1.498588502386111</v>
+        <v>0.2584065515883436</v>
       </c>
       <c r="H20" s="10" t="n">
-        <v>0.1922693789811568</v>
+        <v>-0.1889874153679117</v>
       </c>
       <c r="I20" s="10" t="n">
-        <v>3.556474709924262</v>
+        <v>2.828777895089933</v>
       </c>
       <c r="J20" s="10" t="n">
-        <v>0.05931358103946814</v>
+        <v>0.09258879282334501</v>
       </c>
       <c r="K20" s="10" t="n">
-        <v>1.110582028950847</v>
+        <v>1.386998527756787</v>
       </c>
       <c r="L20" s="11" t="n">
-        <v>0.03341074732726722</v>
+        <v>0.01904206983715261</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="9" t="inlineStr">
         <is>
-          <t>savings.account.and.bonds</t>
+          <t>credit.history</t>
         </is>
       </c>
       <c r="B21" s="10" t="n">
-        <v>0.7523722427881178</v>
+        <v>1.068954377628909</v>
       </c>
       <c r="C21" s="10" t="n">
-        <v>0.2422152960533528</v>
+        <v>0.2488693864508264</v>
       </c>
       <c r="D21" s="10" t="n">
-        <v>3.106212758018357</v>
+        <v>4.295242548203582</v>
       </c>
       <c r="E21" s="10" t="n">
-        <v>0.001895003164807475</v>
+        <v>1.745024430076349e-05</v>
       </c>
       <c r="F21" s="10" t="n">
-        <v>0.2776389860188396</v>
+        <v>0.5811793433307093</v>
       </c>
       <c r="G21" s="10" t="n">
-        <v>1.227105499557396</v>
+        <v>1.55672941192711</v>
       </c>
       <c r="H21" s="10" t="n">
-        <v>0.3386948921280651</v>
+        <v>0.5355885354615743</v>
       </c>
       <c r="I21" s="10" t="n">
-        <v>9.648557698076006</v>
+        <v>18.4491085478984</v>
       </c>
       <c r="J21" s="10" t="n">
-        <v>0.001895003164807476</v>
+        <v>1.74502443007635e-05</v>
       </c>
       <c r="K21" s="10" t="n">
-        <v>1.097554232555197</v>
+        <v>1.450182245015747</v>
       </c>
       <c r="L21" s="11" t="n">
-        <v>0.03909719819184641</v>
+        <v>0.1148494438421855</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="9" t="inlineStr">
         <is>
-          <t>present.employment.since</t>
+          <t>installment.rate.in.percentage.of.disposable.income</t>
         </is>
       </c>
       <c r="B22" s="10" t="n">
-        <v>0.7863547623103803</v>
+        <v>2.319157369285501</v>
       </c>
       <c r="C22" s="10" t="n">
-        <v>0.2442840850796072</v>
+        <v>0.5826144511281193</v>
       </c>
       <c r="D22" s="10" t="n">
-        <v>3.219017571505419</v>
+        <v>3.980603922190576</v>
       </c>
       <c r="E22" s="10" t="n">
-        <v>0.00128630602731157</v>
+        <v>6.874040438078588e-05</v>
       </c>
       <c r="F22" s="10" t="n">
-        <v>0.3075667535580318</v>
+        <v>1.177254028201816</v>
       </c>
       <c r="G22" s="10" t="n">
-        <v>1.265142771062729</v>
+        <v>3.461060710369186</v>
       </c>
       <c r="H22" s="10" t="n">
-        <v>0.2973898976638326</v>
+        <v>0.3980886672786308</v>
       </c>
       <c r="I22" s="10" t="n">
-        <v>10.36207412566064</v>
+        <v>15.845207585359</v>
       </c>
       <c r="J22" s="10" t="n">
-        <v>0.00128630602731157</v>
+        <v>6.874040438078572e-05</v>
       </c>
       <c r="K22" s="10" t="n">
-        <v>1.076530665855001</v>
+        <v>1.078249610457313</v>
       </c>
       <c r="L22" s="11" t="n">
-        <v>0.06371980526187677</v>
+        <v>0.05747143123669587</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="inlineStr">
         <is>
-          <t>duration.in.month</t>
+          <t>housing</t>
         </is>
       </c>
       <c r="B23" s="7" t="n">
-        <v>1.088005930680652</v>
+        <v>0.7280921533066069</v>
       </c>
       <c r="C23" s="7" t="n">
-        <v>0.245408011788501</v>
+        <v>0.2887770099811189</v>
       </c>
       <c r="D23" s="7" t="n">
-        <v>4.43345725655576</v>
+        <v>2.521295422215957</v>
       </c>
       <c r="E23" s="7" t="n">
-        <v>9.27338991455342e-06</v>
+        <v>0.01169236422364248</v>
       </c>
       <c r="F23" s="7" t="n">
-        <v>0.6070150660576086</v>
+        <v>0.16209961418045</v>
       </c>
       <c r="G23" s="7" t="n">
-        <v>1.568996795303695</v>
+        <v>1.294084692432764</v>
       </c>
       <c r="H23" s="7" t="n">
-        <v>0.4483908396565341</v>
+        <v>0.2309302103782693</v>
       </c>
       <c r="I23" s="7" t="n">
-        <v>19.65554324570693</v>
+        <v>6.356930606087142</v>
       </c>
       <c r="J23" s="7" t="n">
-        <v>9.273389914553408e-06</v>
+        <v>0.01169236422364249</v>
       </c>
       <c r="K23" s="7" t="n">
-        <v>1.047968045953181</v>
+        <v>1.037260645787511</v>
       </c>
       <c r="L23" s="8" t="n">
-        <v>0.1343035391517879</v>
+        <v>0.03072099556685252</v>
       </c>
     </row>
     <row r="24">
@@ -1432,47 +1432,47 @@
       <c r="A26" s="9" t="n"/>
       <c r="B26" s="10" t="inlineStr">
         <is>
+          <t>age.in.years</t>
+        </is>
+      </c>
+      <c r="C26" s="10" t="inlineStr">
+        <is>
+          <t>savings.account.and.bonds</t>
+        </is>
+      </c>
+      <c r="D26" s="10" t="inlineStr">
+        <is>
+          <t>credit.amount</t>
+        </is>
+      </c>
+      <c r="E26" s="10" t="inlineStr">
+        <is>
+          <t>purpose</t>
+        </is>
+      </c>
+      <c r="F26" s="10" t="inlineStr">
+        <is>
+          <t>status.of.existing.checking.account</t>
+        </is>
+      </c>
+      <c r="G26" s="10" t="inlineStr">
+        <is>
+          <t>number.of.existing.credits.at.this.bank</t>
+        </is>
+      </c>
+      <c r="H26" s="10" t="inlineStr">
+        <is>
+          <t>credit.history</t>
+        </is>
+      </c>
+      <c r="I26" s="10" t="inlineStr">
+        <is>
+          <t>installment.rate.in.percentage.of.disposable.income</t>
+        </is>
+      </c>
+      <c r="J26" s="10" t="inlineStr">
+        <is>
           <t>housing</t>
-        </is>
-      </c>
-      <c r="C26" s="10" t="inlineStr">
-        <is>
-          <t>status.of.existing.checking.account</t>
-        </is>
-      </c>
-      <c r="D26" s="10" t="inlineStr">
-        <is>
-          <t>installment.rate.in.percentage.of.disposable.income</t>
-        </is>
-      </c>
-      <c r="E26" s="10" t="inlineStr">
-        <is>
-          <t>purpose</t>
-        </is>
-      </c>
-      <c r="F26" s="10" t="inlineStr">
-        <is>
-          <t>credit.amount</t>
-        </is>
-      </c>
-      <c r="G26" s="10" t="inlineStr">
-        <is>
-          <t>age.in.years</t>
-        </is>
-      </c>
-      <c r="H26" s="10" t="inlineStr">
-        <is>
-          <t>savings.account.and.bonds</t>
-        </is>
-      </c>
-      <c r="I26" s="10" t="inlineStr">
-        <is>
-          <t>present.employment.since</t>
-        </is>
-      </c>
-      <c r="J26" s="10" t="inlineStr">
-        <is>
-          <t>duration.in.month</t>
         </is>
       </c>
       <c r="K26" s="10" t="n"/>
@@ -1481,35 +1481,35 @@
     <row r="27">
       <c r="A27" s="9" t="inlineStr">
         <is>
-          <t>housing</t>
+          <t>age.in.years</t>
         </is>
       </c>
       <c r="B27" s="10" t="n">
         <v>1</v>
       </c>
       <c r="C27" s="10" t="n">
-        <v>0.0885418563198889</v>
+        <v>0.1691647458415965</v>
       </c>
       <c r="D27" s="10" t="n">
-        <v>-0.07502821984938983</v>
+        <v>-0.008082454746586986</v>
       </c>
       <c r="E27" s="10" t="n">
-        <v>0.0673520774367473</v>
+        <v>-0.09563437768939444</v>
       </c>
       <c r="F27" s="10" t="n">
-        <v>0.06449482878665802</v>
+        <v>0.063536396449064</v>
       </c>
       <c r="G27" s="10" t="n">
-        <v>-0.01728566064249711</v>
+        <v>0.1112073086191369</v>
       </c>
       <c r="H27" s="10" t="n">
-        <v>-0.01595253207654717</v>
+        <v>0.1656247172953032</v>
       </c>
       <c r="I27" s="10" t="n">
-        <v>0.06505946756578647</v>
+        <v>-0.05993917998353979</v>
       </c>
       <c r="J27" s="10" t="n">
-        <v>0.05306271581819098</v>
+        <v>0.03315631789445925</v>
       </c>
       <c r="K27" s="10" t="n"/>
       <c r="L27" s="11" t="n"/>
@@ -1517,35 +1517,35 @@
     <row r="28">
       <c r="A28" s="9" t="inlineStr">
         <is>
-          <t>status.of.existing.checking.account</t>
+          <t>savings.account.and.bonds</t>
         </is>
       </c>
       <c r="B28" s="10" t="n">
-        <v>0.0885418563198889</v>
+        <v>0.1691647458415965</v>
       </c>
       <c r="C28" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="10" t="n">
-        <v>-0.001523283612969293</v>
+        <v>-0.03726907589107842</v>
       </c>
       <c r="E28" s="10" t="n">
-        <v>0.1287117955384501</v>
+        <v>0.09888115153584234</v>
       </c>
       <c r="F28" s="10" t="n">
-        <v>0.007946881904132945</v>
+        <v>0.2116044449927929</v>
       </c>
       <c r="G28" s="10" t="n">
-        <v>0.1009718767228579</v>
+        <v>-0.02013455491415136</v>
       </c>
       <c r="H28" s="10" t="n">
-        <v>0.2340676423397493</v>
+        <v>0.0456743550918136</v>
       </c>
       <c r="I28" s="10" t="n">
-        <v>0.1440912637711744</v>
+        <v>-0.08110218812916567</v>
       </c>
       <c r="J28" s="10" t="n">
-        <v>0.01085633897192569</v>
+        <v>-0.003039325552784339</v>
       </c>
       <c r="K28" s="10" t="n"/>
       <c r="L28" s="11" t="n"/>
@@ -1553,35 +1553,35 @@
     <row r="29">
       <c r="A29" s="9" t="inlineStr">
         <is>
-          <t>installment.rate.in.percentage.of.disposable.income</t>
+          <t>credit.amount</t>
         </is>
       </c>
       <c r="B29" s="10" t="n">
-        <v>-0.07502821984938983</v>
+        <v>-0.008082454746586986</v>
       </c>
       <c r="C29" s="10" t="n">
-        <v>-0.001523283612969293</v>
+        <v>-0.03726907589107842</v>
       </c>
       <c r="D29" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E29" s="10" t="n">
-        <v>-0.01932330615872743</v>
+        <v>-0.008921245233343556</v>
       </c>
       <c r="F29" s="10" t="n">
-        <v>-0.07826539155993008</v>
+        <v>0.02832376597597611</v>
       </c>
       <c r="G29" s="10" t="n">
-        <v>-0.0423449693996718</v>
+        <v>-0.01059439153511781</v>
       </c>
       <c r="H29" s="10" t="n">
-        <v>-0.08311536410199402</v>
+        <v>0.05721052196072506</v>
       </c>
       <c r="I29" s="10" t="n">
-        <v>-0.04845250709467129</v>
+        <v>-0.2311195932916181</v>
       </c>
       <c r="J29" s="10" t="n">
-        <v>0.07447178225894761</v>
+        <v>0.04632715628215875</v>
       </c>
       <c r="K29" s="10" t="n"/>
       <c r="L29" s="11" t="n"/>
@@ -1593,31 +1593,31 @@
         </is>
       </c>
       <c r="B30" s="10" t="n">
-        <v>0.0673520774367473</v>
+        <v>-0.09563437768939444</v>
       </c>
       <c r="C30" s="10" t="n">
-        <v>0.1287117955384501</v>
+        <v>0.09888115153584234</v>
       </c>
       <c r="D30" s="10" t="n">
-        <v>-0.01932330615872743</v>
+        <v>-0.008921245233343556</v>
       </c>
       <c r="E30" s="10" t="n">
         <v>1</v>
       </c>
       <c r="F30" s="10" t="n">
-        <v>0.04887205957967239</v>
+        <v>0.1389681790903947</v>
       </c>
       <c r="G30" s="10" t="n">
-        <v>-0.110761215788963</v>
+        <v>-0.04577341403247482</v>
       </c>
       <c r="H30" s="10" t="n">
-        <v>0.0699342274830794</v>
+        <v>-0.03469135884786096</v>
       </c>
       <c r="I30" s="10" t="n">
-        <v>0.04444642882022483</v>
+        <v>-0.02251654888399932</v>
       </c>
       <c r="J30" s="10" t="n">
-        <v>-0.1047233517431374</v>
+        <v>0.07187817478496603</v>
       </c>
       <c r="K30" s="10" t="n"/>
       <c r="L30" s="11" t="n"/>
@@ -1625,35 +1625,35 @@
     <row r="31">
       <c r="A31" s="9" t="inlineStr">
         <is>
-          <t>credit.amount</t>
+          <t>status.of.existing.checking.account</t>
         </is>
       </c>
       <c r="B31" s="10" t="n">
-        <v>0.06449482878665802</v>
+        <v>0.063536396449064</v>
       </c>
       <c r="C31" s="10" t="n">
-        <v>0.007946881904132945</v>
+        <v>0.2116044449927929</v>
       </c>
       <c r="D31" s="10" t="n">
-        <v>-0.07826539155993008</v>
+        <v>0.02832376597597611</v>
       </c>
       <c r="E31" s="10" t="n">
-        <v>0.04887205957967239</v>
+        <v>0.1389681790903947</v>
       </c>
       <c r="F31" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G31" s="10" t="n">
-        <v>-0.08336526733463774</v>
+        <v>0.1276676663656884</v>
       </c>
       <c r="H31" s="10" t="n">
-        <v>-0.002400722205969198</v>
+        <v>0.1977270731397576</v>
       </c>
       <c r="I31" s="10" t="n">
-        <v>-0.01976079057030413</v>
+        <v>-0.01732810293364445</v>
       </c>
       <c r="J31" s="10" t="n">
-        <v>0.08784857212878731</v>
+        <v>0.1304357356469764</v>
       </c>
       <c r="K31" s="10" t="n"/>
       <c r="L31" s="11" t="n"/>
@@ -1661,35 +1661,35 @@
     <row r="32">
       <c r="A32" s="9" t="inlineStr">
         <is>
-          <t>age.in.years</t>
+          <t>number.of.existing.credits.at.this.bank</t>
         </is>
       </c>
       <c r="B32" s="10" t="n">
-        <v>-0.01728566064249711</v>
+        <v>0.1112073086191369</v>
       </c>
       <c r="C32" s="10" t="n">
-        <v>0.1009718767228579</v>
+        <v>-0.02013455491415136</v>
       </c>
       <c r="D32" s="10" t="n">
-        <v>-0.0423449693996718</v>
+        <v>-0.01059439153511781</v>
       </c>
       <c r="E32" s="10" t="n">
-        <v>-0.110761215788963</v>
+        <v>-0.04577341403247482</v>
       </c>
       <c r="F32" s="10" t="n">
-        <v>-0.08336526733463774</v>
+        <v>0.1276676663656884</v>
       </c>
       <c r="G32" s="10" t="n">
         <v>1</v>
       </c>
       <c r="H32" s="10" t="n">
-        <v>0.1513178431552293</v>
+        <v>0.5212495895656725</v>
       </c>
       <c r="I32" s="10" t="n">
-        <v>0.2066659725406873</v>
+        <v>-0.05210897347680796</v>
       </c>
       <c r="J32" s="10" t="n">
-        <v>0.1210619284143789</v>
+        <v>0.04963645045676171</v>
       </c>
       <c r="K32" s="10" t="n"/>
       <c r="L32" s="11" t="n"/>
@@ -1697,35 +1697,35 @@
     <row r="33">
       <c r="A33" s="9" t="inlineStr">
         <is>
-          <t>savings.account.and.bonds</t>
+          <t>credit.history</t>
         </is>
       </c>
       <c r="B33" s="10" t="n">
-        <v>-0.01595253207654717</v>
+        <v>0.1656247172953032</v>
       </c>
       <c r="C33" s="10" t="n">
-        <v>0.2340676423397493</v>
+        <v>0.0456743550918136</v>
       </c>
       <c r="D33" s="10" t="n">
-        <v>-0.08311536410199402</v>
+        <v>0.05721052196072506</v>
       </c>
       <c r="E33" s="10" t="n">
-        <v>0.0699342274830794</v>
+        <v>-0.03469135884786096</v>
       </c>
       <c r="F33" s="10" t="n">
-        <v>-0.002400722205969198</v>
+        <v>0.1977270731397576</v>
       </c>
       <c r="G33" s="10" t="n">
-        <v>0.1513178431552293</v>
+        <v>0.5212495895656725</v>
       </c>
       <c r="H33" s="10" t="n">
         <v>1</v>
       </c>
       <c r="I33" s="10" t="n">
-        <v>0.1364706466193921</v>
+        <v>-0.08863989519513137</v>
       </c>
       <c r="J33" s="10" t="n">
-        <v>-0.02636143010881219</v>
+        <v>0.1172495064360057</v>
       </c>
       <c r="K33" s="10" t="n"/>
       <c r="L33" s="11" t="n"/>
@@ -1733,35 +1733,35 @@
     <row r="34">
       <c r="A34" s="9" t="inlineStr">
         <is>
-          <t>present.employment.since</t>
+          <t>installment.rate.in.percentage.of.disposable.income</t>
         </is>
       </c>
       <c r="B34" s="10" t="n">
-        <v>0.06505946756578647</v>
+        <v>-0.05993917998353979</v>
       </c>
       <c r="C34" s="10" t="n">
-        <v>0.1440912637711744</v>
+        <v>-0.08110218812916567</v>
       </c>
       <c r="D34" s="10" t="n">
-        <v>-0.04845250709467129</v>
+        <v>-0.2311195932916181</v>
       </c>
       <c r="E34" s="10" t="n">
-        <v>0.04444642882022483</v>
+        <v>-0.02251654888399932</v>
       </c>
       <c r="F34" s="10" t="n">
-        <v>-0.01976079057030413</v>
+        <v>-0.01732810293364445</v>
       </c>
       <c r="G34" s="10" t="n">
-        <v>0.2066659725406873</v>
+        <v>-0.05210897347680796</v>
       </c>
       <c r="H34" s="10" t="n">
-        <v>0.1364706466193921</v>
+        <v>-0.08863989519513137</v>
       </c>
       <c r="I34" s="10" t="n">
         <v>1</v>
       </c>
       <c r="J34" s="10" t="n">
-        <v>0.009984208343368132</v>
+        <v>-0.07199134510798434</v>
       </c>
       <c r="K34" s="10" t="n"/>
       <c r="L34" s="11" t="n"/>
@@ -1769,32 +1769,32 @@
     <row r="35">
       <c r="A35" s="12" t="inlineStr">
         <is>
-          <t>duration.in.month</t>
+          <t>housing</t>
         </is>
       </c>
       <c r="B35" s="13" t="n">
-        <v>0.05306271581819098</v>
+        <v>0.03315631789445925</v>
       </c>
       <c r="C35" s="13" t="n">
-        <v>0.01085633897192569</v>
+        <v>-0.003039325552784339</v>
       </c>
       <c r="D35" s="13" t="n">
-        <v>0.07447178225894761</v>
+        <v>0.04632715628215875</v>
       </c>
       <c r="E35" s="13" t="n">
-        <v>-0.1047233517431374</v>
+        <v>0.07187817478496603</v>
       </c>
       <c r="F35" s="13" t="n">
-        <v>0.08784857212878731</v>
+        <v>0.1304357356469764</v>
       </c>
       <c r="G35" s="13" t="n">
-        <v>0.1210619284143789</v>
+        <v>0.04963645045676171</v>
       </c>
       <c r="H35" s="13" t="n">
-        <v>-0.02636143010881219</v>
+        <v>0.1172495064360057</v>
       </c>
       <c r="I35" s="13" t="n">
-        <v>0.009984208343368132</v>
+        <v>-0.07199134510798434</v>
       </c>
       <c r="J35" s="13" t="n">
         <v>1</v>

</xml_diff>